<commit_message>
got working code for isolating both name and ability and can push that to excel bypassing the dictionary
</commit_message>
<xml_diff>
--- a/day_2/output.xlsx
+++ b/day_2/output.xlsx
@@ -1,43 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\dkayzee\vit\intro-python-august-2021\itp_week_4\day_2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE1364D1-5557-4725-962A-E4ADEF91677F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="4590" windowWidth="28800" windowHeight="15435" xr2:uid="{B9C8922C-22A4-4A82-B087-2D280D427692}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-26760" yWindow="1590" windowWidth="23040" windowHeight="12360" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -56,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -370,13 +419,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDF1B2C-A62F-460C-B79F-11C4A14BEEEE}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="A1:D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="15.42578125" bestFit="1" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Ability</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>bulbasaur</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>overgrow</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ivysaur</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>overgrow</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>venusaur</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>overgrow</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>charmander</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>blaze</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>charmeleon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>blaze</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>charizard</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>blaze</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>squirtle</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>torrent</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>wartortle</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>torrent</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>blastoise</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>torrent</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>caterpie</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>shield-dust</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>metapod</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>shed-skin</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>butterfree</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>compound-eyes</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>weedle</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>shield-dust</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>kakuna</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>shed-skin</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>beedrill</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>swarm</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>pidgey</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>keen-eye</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>pidgeotto</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>keen-eye</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>pidgeot</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>keen-eye</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>rattata</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>run-away</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>raticate</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>run-away</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>